<commit_message>
manufacturing data prepped for Newbury
</commit_message>
<xml_diff>
--- a/design_files/worklib/pc065b_fibv2_toplevel/physical/manufacture 2024/bill of materials.xlsx
+++ b/design_files/worklib/pc065b_fibv2_toplevel/physical/manufacture 2024/bill of materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ppfs6.physics.ox.ac.uk\CEG\Central Electronics\Projects\Hastingsp\DUNE\uob-hep-pc065\design_files\worklib\pc065b_fibv2_toplevel\physical\manufacture 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D1667F-F69E-4C88-B7AE-EA802ABDAB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F24BD3-F456-428A-BC77-80DFD1D61A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16650" yWindow="2790" windowWidth="28800" windowHeight="15345" xr2:uid="{F89D0B4F-2DBE-4679-BEF7-16FC5DEE2B0A}"/>
+    <workbookView xWindow="8490" yWindow="1650" windowWidth="28800" windowHeight="15345" xr2:uid="{F89D0B4F-2DBE-4679-BEF7-16FC5DEE2B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB52B35-0EB8-4FBE-95A0-CA35294B5EBC}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>